<commit_message>
added related work section
</commit_message>
<xml_diff>
--- a/FinalReport/key_tables.xlsx
+++ b/FinalReport/key_tables.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g_gna\Documents\TCD\Modules\CS7CS5_Dissertation\FinalReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9355CB-6CBE-4FAA-8FAC-4E3163E31E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2D95B9-91C3-4401-9512-813ECC6B5AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9463" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9463" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="env_vars" sheetId="1" r:id="rId1"/>
-    <sheet name="ui_components" sheetId="2" r:id="rId2"/>
-    <sheet name="data" sheetId="3" r:id="rId3"/>
-    <sheet name="sim mw games key ideas" sheetId="4" r:id="rId4"/>
-    <sheet name="pedagogy best practices" sheetId="5" r:id="rId5"/>
-    <sheet name="challenges" sheetId="6" r:id="rId6"/>
+    <sheet name="tool_critique" sheetId="8" r:id="rId1"/>
+    <sheet name="env_vars" sheetId="1" r:id="rId2"/>
+    <sheet name="ui_components" sheetId="2" r:id="rId3"/>
+    <sheet name="data" sheetId="3" r:id="rId4"/>
+    <sheet name="sim mw games key ideas" sheetId="4" r:id="rId5"/>
+    <sheet name="pedagogy best practices" sheetId="5" r:id="rId6"/>
+    <sheet name="challenges" sheetId="6" r:id="rId7"/>
+    <sheet name="tool_pros_cons" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="230">
   <si>
     <t>Carbon Dynamics</t>
   </si>
@@ -563,12 +565,337 @@
   <si>
     <t>Challenge 5</t>
   </si>
+  <si>
+    <t>Pros</t>
+  </si>
+  <si>
+    <t>Cons</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tool is very </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>flexible</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and supports a rich variety of scenarios. Participants can come up with creative strategies not severely limited by tool capabilities.</t>
+    </r>
+  </si>
+  <si>
+    <t>Participants enjoyed the ComMod wherein decisions followed group discussions.</t>
+  </si>
+  <si>
+    <t>Participants found the UI too mathematical and hard to relate to.</t>
+  </si>
+  <si>
+    <t>Participants cannot interact with the tool directly. They must rely on the facilitator.</t>
+  </si>
+  <si>
+    <t>Tool requires extensive introductory training and user guides.</t>
+  </si>
+  <si>
+    <t>Tool use instructional material (2 usage videos, 6 booklets one for each role + facilitator) provided was overwhelming for some participants. Thus, learning curve is very high.</t>
+  </si>
+  <si>
+    <t>This tool requires an elaborate set up with 2 projectors and a facilitator. It was built using software that needs to be downloaded and installed along with associated user guide materials. This makes this tool less accessible.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tool is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>realistic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> with well a designed ABM.</t>
+    </r>
+  </si>
+  <si>
+    <t>Foster Forest</t>
+  </si>
+  <si>
+    <t>Participants must be familiar with the domain. Not for the lay man.</t>
+  </si>
+  <si>
+    <t>Participants appreciated being able to test strategies in a risk-free environment.</t>
+  </si>
+  <si>
+    <t>Mine Set</t>
+  </si>
+  <si>
+    <t>ComMod.</t>
+  </si>
+  <si>
+    <t>Models a rich variety of land use change drivers.</t>
+  </si>
+  <si>
+    <t>Allegorical model is less scientifically accurate.</t>
+  </si>
+  <si>
+    <t>Significant set up required.</t>
+  </si>
+  <si>
+    <t>Engaging and immersive.</t>
+  </si>
+  <si>
+    <t>No explicit mention of climate change.</t>
+  </si>
+  <si>
+    <t>Incorporates model progression to gradually reveal game complexity.</t>
+  </si>
+  <si>
+    <t>Caters to a wide audience, particularly forest stakeholders. However, non-expert audiences can also enjoy and learn from it.</t>
+  </si>
+  <si>
+    <t>The physical mine set board game is a more holistic visceral experince that is more likely to be remembered given close in-person interaction with peers and physical interaction with game pieces.</t>
+  </si>
+  <si>
+    <t>The physical nature of the game requires in-person attendance. This makes it less widely accessible unless online collaborative tools (like zoom, google meet, etc.) are incorporated and a third party coordinates and communicates all player moves. This is tedious.</t>
+  </si>
+  <si>
+    <t>About That Forest</t>
+  </si>
+  <si>
+    <t>Engaging.</t>
+  </si>
+  <si>
+    <t>Competition in addition to cooperation.</t>
+  </si>
+  <si>
+    <t>Widely accessible.</t>
+  </si>
+  <si>
+    <t>Appeals to a wide age group and range of starting knowledge levels.</t>
+  </si>
+  <si>
+    <t>Underlying model and research not openly available.</t>
+  </si>
+  <si>
+    <t>Atmospheric CO2 levels is not a modelled indcator.</t>
+  </si>
+  <si>
+    <t>No big cons.</t>
+  </si>
+  <si>
+    <t>Multiple economic drivers of exploitation.</t>
+  </si>
+  <si>
+    <t>Underlying code allows for easily modifiable settings.</t>
+  </si>
+  <si>
+    <t>Forest Kids</t>
+  </si>
+  <si>
+    <t>Motivating mini-games.</t>
+  </si>
+  <si>
+    <t>Visually very attractive.</t>
+  </si>
+  <si>
+    <t>In-app help is well placed and provided in small, easy to absorb chunks.</t>
+  </si>
+  <si>
+    <t>Great user experience with smooth interactions.</t>
+  </si>
+  <si>
+    <t>Very informative and covers different topics related to forest biodiversity and Earth's climate.</t>
+  </si>
+  <si>
+    <t>Text in the game is supported by audio readouts to make it easier to absorb for children.</t>
+  </si>
+  <si>
+    <t>Facts are repeated from time to time but not too frequently.  This may promote information persistence in memory.</t>
+  </si>
+  <si>
+    <t>Age appropriate for children.</t>
+  </si>
+  <si>
+    <t>Facts presented during matching and memory  games are random and lack connection. This can make them hard to learn.</t>
+  </si>
+  <si>
+    <t>No learning through making.</t>
+  </si>
+  <si>
+    <t>Games are very engaging. The timing element adds a sense of urgency. As pointed out by [], games that are very competative or engaging, often with a scoring mechanism, especially in the absence of constructionist mechanisms, can significantly effect learning negatively. Users tend to enter a "twitch" mode where they are hyperfocused on improving score and learning suffers. This is a real threat in this game. Personally, when trying the memory game, I soon found myself ignoring the facts as I focused more on memorizing tile symbols to get the matches right before the timer runs out to score maximum points.</t>
+  </si>
+  <si>
+    <t>SimForest</t>
+  </si>
+  <si>
+    <t>Rich set of manipulatable controls.</t>
+  </si>
+  <si>
+    <t>Allows moving through times at various speeds.</t>
+  </si>
+  <si>
+    <t>Good data visualization.</t>
+  </si>
+  <si>
+    <t>Does not consider atmospheric CO2 levels.</t>
+  </si>
+  <si>
+    <t>Only available on PC and requires download and possibly some set up (OS, Java, or Swing related compatibility issues possible).</t>
+  </si>
+  <si>
+    <t>Can be adapted to teach a range of age groups and expertise levels (school grade 4 all the way up to university graduate students and forestry professionals).</t>
+  </si>
+  <si>
+    <t>General forest growth simulation around which multiple learning scenarios may be developed.</t>
+  </si>
+  <si>
+    <t>Facilitates  inquiry-based  constructivist learning comprising multiple iterative inquiry cycles with steps (i) ask question or form hypothesis, (ii) plan to answer or test hypothesis (iii) note observations, (iv) analyze data gathered, (v) communicate learnings.</t>
+  </si>
+  <si>
+    <t>Clean user-friendly UI.</t>
+  </si>
+  <si>
+    <t>Allows multi-level control (high-level or black box, as well as low-level or glass box).</t>
+  </si>
+  <si>
+    <t>Does not consider economic value of forests.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INFORMATIVE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TOOL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> →
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>QUALITY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ↓</t>
+    </r>
+  </si>
+  <si>
+    <t>FOSTER FOREST</t>
+  </si>
+  <si>
+    <t>MINE SET</t>
+  </si>
+  <si>
+    <t>ABOUT 
+THAT FOREST</t>
+  </si>
+  <si>
+    <t>FOREST KIDS</t>
+  </si>
+  <si>
+    <t>MYCROFOREST</t>
+  </si>
+  <si>
+    <t>ENGAGING</t>
+  </si>
+  <si>
+    <t>EASILY ACCESSIBLE</t>
+  </si>
+  <si>
+    <t>FOR YOUTH</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>SOLO</t>
+  </si>
+  <si>
+    <t>FOCUSED AIM</t>
+  </si>
+  <si>
+    <t>FOREST MANAGEMENT</t>
+  </si>
+  <si>
+    <t>FOREST AS CARBON SINK</t>
+  </si>
+  <si>
+    <t>FINANCIAL MOTIVE</t>
+  </si>
+  <si>
+    <t>LOW ENTRY THRESHOLD</t>
+  </si>
+  <si>
+    <t>EASY TO USE UI</t>
+  </si>
+  <si>
+    <t>SUFFICIENT BUILT IN HELP</t>
+  </si>
+  <si>
+    <t>SIMFOREST</t>
+  </si>
+  <si>
+    <t>⚫</t>
+  </si>
+  <si>
+    <t>REALISTIC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,8 +950,45 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -727,8 +1091,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE1E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -859,11 +1247,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -956,6 +1355,81 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1016,65 +1490,47 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1369,6 +1825,347 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9079DD0-448F-48EB-B592-370B7EA5A551}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="23.921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="13.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A1" s="90" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="88" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="88" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="88" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="88" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="88" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="87" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="89" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="88" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="88" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="G5" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="88" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="87" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" s="87" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="88" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G8" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="88" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="F9" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G9" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="88" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="E10" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="88" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G11" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="88" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="G12" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="G13" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="88" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="E14" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G14" s="86" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
@@ -1387,19 +2184,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="58"/>
       <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="84.9" x14ac:dyDescent="0.4">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="60"/>
       <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
@@ -1407,8 +2204,8 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1416,8 +2213,8 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="118.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1445,19 +2242,19 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="42.45" x14ac:dyDescent="0.4">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="41"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
@@ -1474,7 +2271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60BA77A-0FF7-4A09-AAA8-E53725F430B2}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1596,7 +2393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5009B86D-BF46-461E-BF16-B020EE8D75CF}">
   <dimension ref="A1:S15"/>
   <sheetViews>
@@ -1672,12 +2469,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
       <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -1741,12 +2538,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="23.15" x14ac:dyDescent="0.4">
@@ -1810,12 +2607,12 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
     </row>
     <row r="13" spans="1:7" ht="23.15" x14ac:dyDescent="0.4">
       <c r="A13" s="22" t="s">
@@ -1888,7 +2685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F247DBC2-86D7-40D9-BBB1-B4B3735D2E61}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1906,56 +2703,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="56.6" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="71" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="73" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="70.75" x14ac:dyDescent="0.35">
-      <c r="A2" s="47"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="49"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="74"/>
     </row>
     <row r="3" spans="1:4" ht="42.45" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="28" t="s">
         <v>92</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="75" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="70.75" x14ac:dyDescent="0.35">
-      <c r="A4" s="47"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="76"/>
     </row>
     <row r="5" spans="1:4" ht="70.75" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="51"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1970,7 +2767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FE6774-1E3A-4B01-9F79-0CE882F43062}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -1985,10 +2782,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="33" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2017,7 +2814,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="34" t="s">
         <v>101</v>
       </c>
       <c r="B5" s="28" t="s">
@@ -2028,7 +2825,7 @@
       <c r="A6" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="77" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2036,7 +2833,7 @@
       <c r="A7" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="55"/>
+      <c r="B7" s="77"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="29" t="s">
@@ -2050,7 +2847,7 @@
       <c r="A9" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="77" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2058,7 +2855,7 @@
       <c r="A10" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="55"/>
+      <c r="B10" s="77"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="29" t="s">
@@ -2072,7 +2869,7 @@
       <c r="A12" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="77" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2080,7 +2877,7 @@
       <c r="A13" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="55"/>
+      <c r="B13" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2092,39 +2889,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47BAC5F-10D1-4E9A-81F4-B6DA49B47F0B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.3046875" style="60" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.3046875" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="30.69140625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="30.69140625" style="56" customWidth="1"/>
-    <col min="6" max="16384" width="9.23046875" style="56"/>
+    <col min="5" max="5" width="30.69140625" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="9.23046875" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" s="59"/>
-      <c r="B1" s="57" t="s">
+      <c r="A1" s="38"/>
+      <c r="B1" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="37" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="113.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="50" t="s">
         <v>146</v>
       </c>
       <c r="B2" s="29" t="s">
@@ -2141,13 +2938,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="240.45" x14ac:dyDescent="0.4">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="49" t="s">
         <v>147</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="43" t="s">
         <v>129</v>
       </c>
       <c r="D3" s="31" t="s">
@@ -2158,13 +2955,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="99" x14ac:dyDescent="0.4">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="48" t="s">
         <v>148</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="40" t="s">
         <v>130</v>
       </c>
       <c r="D4" s="28" t="s">
@@ -2175,40 +2972,405 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="183.9" x14ac:dyDescent="0.4">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="41" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="169.75" x14ac:dyDescent="0.4">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="44" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E372F1-BAA7-4FDD-A770-A93F85875E6A}">
+  <dimension ref="A1:N45"/>
+  <sheetViews>
+    <sheetView topLeftCell="M40" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43:N45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.69140625" style="51" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.69140625" style="51" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.69140625" style="26" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="40.69140625" style="56" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.69140625" style="56" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="2.69140625" style="26" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="50.69140625" style="56" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="20.69140625" style="56" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="2.69140625" style="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="30.69140625" style="56" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="40.69140625" style="56" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.69140625" style="26" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="50.69140625" style="56" customWidth="1"/>
+    <col min="14" max="14" width="20.69140625" style="56" customWidth="1"/>
+    <col min="15" max="16384" width="9.23046875" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="81" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="83"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="A3" s="82" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="A4" s="82"/>
+      <c r="B4" s="55" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="A5" s="82"/>
+      <c r="B5" s="55" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="A6" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="56.6" x14ac:dyDescent="0.35">
+      <c r="A7" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="70.75" x14ac:dyDescent="0.35">
+      <c r="A8" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="81" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="83"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="82" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D12" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="82"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="D13" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="D14" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="42.45" x14ac:dyDescent="0.35">
+      <c r="D15" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="82" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="70.75" x14ac:dyDescent="0.35">
+      <c r="D16" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="E16" s="82"/>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G17" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="H17" s="81"/>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G18" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="H19" s="55" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G20" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="H20" s="82" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G21" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="82"/>
+    </row>
+    <row r="22" spans="7:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="H22" s="82"/>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G23" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H23" s="82" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G24" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="H24" s="82"/>
+    </row>
+    <row r="25" spans="7:11" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="G25" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="H25" s="82"/>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="J26" s="81" t="s">
+        <v>185</v>
+      </c>
+      <c r="K26" s="81"/>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="J27" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="K27" s="54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="J28" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="K28" s="55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="J29" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="K29" s="82" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="7:11" ht="28.3" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J30" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="K30" s="82"/>
+    </row>
+    <row r="31" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="J31" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="K31" s="82" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="7:11" ht="42.45" x14ac:dyDescent="0.35">
+      <c r="J32" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="K32" s="82"/>
+    </row>
+    <row r="33" spans="10:14" ht="42.45" x14ac:dyDescent="0.35">
+      <c r="J33" s="55" t="s">
+        <v>188</v>
+      </c>
+      <c r="K33" s="82"/>
+    </row>
+    <row r="34" spans="10:14" ht="42.45" x14ac:dyDescent="0.35">
+      <c r="J34" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="K34" s="82"/>
+    </row>
+    <row r="35" spans="10:14" ht="56.6" x14ac:dyDescent="0.35">
+      <c r="J35" s="55" t="s">
+        <v>192</v>
+      </c>
+      <c r="K35" s="82"/>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="M36" s="81" t="s">
+        <v>197</v>
+      </c>
+      <c r="N36" s="81"/>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="M37" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="N37" s="54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="M38" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="N38" s="55" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="M39" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="N39" s="82" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="10:14" ht="42.45" x14ac:dyDescent="0.35">
+      <c r="M40" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="N40" s="82"/>
+    </row>
+    <row r="41" spans="10:14" ht="70.75" x14ac:dyDescent="0.35">
+      <c r="M41" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="N41" s="82" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="M42" s="55" t="s">
+        <v>206</v>
+      </c>
+      <c r="N42" s="82"/>
+    </row>
+    <row r="43" spans="10:14" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M43" s="55" t="s">
+        <v>199</v>
+      </c>
+      <c r="N43" s="78" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="M44" s="55" t="s">
+        <v>200</v>
+      </c>
+      <c r="N44" s="79"/>
+    </row>
+    <row r="45" spans="10:14" ht="28.3" x14ac:dyDescent="0.35">
+      <c r="M45" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="N45" s="80"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="N43:N45"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="K31:K35"/>
+    <mergeCell ref="K29:K30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>